<commit_message>
2028. Find Missing Observations
</commit_message>
<xml_diff>
--- a/LeetCode/Daily_Challenege/September_2024/Daily september challenge.xlsx
+++ b/LeetCode/Daily_Challenege/September_2024/Daily september challenge.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shubhamrathod/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shubhamrathod/Documents/Study Material/DS/DataStructure-And-Algorithm/LeetCode/Daily_Challenege/September_2024/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EAF627E-7AFC-C244-A935-5B72C54DEFC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D94814A-601D-374C-A740-50F4660F1686}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="46100" yWindow="7660" windowWidth="28040" windowHeight="16340" xr2:uid="{27093052-BF5C-A744-B01C-25DD532CC657}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>September 2024 Daily Challenge</t>
   </si>
@@ -104,12 +104,58 @@
 remaining chalk = k % sum of array.</t>
     </r>
   </si>
+  <si>
+    <t>3. 1945. Sum of Digits of String After Convert</t>
+  </si>
+  <si>
+    <t># Main idea revolves around typecasting
+Convert Str -&gt; Int
+int -&gt; Str</t>
+  </si>
+  <si>
+    <t>4. 874. Walking Robot Simulation</t>
+  </si>
+  <si>
+    <t>the idea is to understand how rotation works.
+Basically look right is nothing but moving one position right -&gt; +1
+look left is nothing but moving one position left -&gt; -1</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=86yKkaNi3sU</t>
+  </si>
+  <si>
+    <t>5. 2028. Find Missing Observations</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Aptos Narrow (Body)"/>
+      </rPr>
+      <t>Math Simulation Problem</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Make sure the dice values are between 1- 6</t>
+    </r>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=yZAA05wKy8Y&amp;t=655s</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -121,6 +167,14 @@
       <sz val="12"/>
       <color rgb="FFFF0000"/>
       <name val="Aptos Narrow (Body)"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -140,21 +194,28 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -487,51 +548,86 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB7E3421-3FED-6D45-9062-E34708192987}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="45" style="4" customWidth="1"/>
-    <col min="2" max="2" width="86.5" style="3" customWidth="1"/>
+    <col min="1" max="1" width="45" style="2" customWidth="1"/>
+    <col min="2" max="2" width="86.5" customWidth="1"/>
+    <col min="3" max="3" width="61.1640625" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="34" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
+    <row r="2" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="68" x14ac:dyDescent="0.2">
-      <c r="B4" s="2" t="s">
+    <row r="4" spans="1:3" ht="68" x14ac:dyDescent="0.2">
+      <c r="B4" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B5" s="2"/>
-    </row>
-    <row r="6" spans="1:2" ht="136" x14ac:dyDescent="0.2">
-      <c r="A6" s="4" t="s">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B5" s="1"/>
+    </row>
+    <row r="6" spans="1:3" ht="136" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="1" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:XFD1"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="C12" r:id="rId1" xr:uid="{D14FDEA8-2424-A24D-B339-CDB437F1A229}"/>
+    <hyperlink ref="C10" r:id="rId2" xr:uid="{F3EFF2F4-F996-1F4D-89FF-4A26296D4786}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
2807. Insert Greatest Common Divisors in Linked List
</commit_message>
<xml_diff>
--- a/LeetCode/Daily_Challenege/September_2024/Daily september challenge.xlsx
+++ b/LeetCode/Daily_Challenege/September_2024/Daily september challenge.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shubhamrathod/Documents/Study Material/DS/DataStructure-And-Algorithm/LeetCode/Daily_Challenege/September_2024/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D94814A-601D-374C-A740-50F4660F1686}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57430365-D0FC-6146-BF7E-CBB42F67E543}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="46100" yWindow="7660" windowWidth="28040" windowHeight="16340" xr2:uid="{27093052-BF5C-A744-B01C-25DD532CC657}"/>
+    <workbookView xWindow="42360" yWindow="6500" windowWidth="28040" windowHeight="16340" xr2:uid="{27093052-BF5C-A744-B01C-25DD532CC657}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>September 2024 Daily Challenge</t>
   </si>
@@ -149,6 +149,21 @@
   </si>
   <si>
     <t>https://www.youtube.com/watch?v=yZAA05wKy8Y&amp;t=655s</t>
+  </si>
+  <si>
+    <t>6. 3217. Delete Nodes From Linked List Present in Array</t>
+  </si>
+  <si>
+    <t>7. 1367. Linked List in Binary Tree</t>
+  </si>
+  <si>
+    <t>8. 725. Split Linked List in Parts</t>
+  </si>
+  <si>
+    <t>9. 2326. Spiral Matrix IV</t>
+  </si>
+  <si>
+    <t>Just like spiral matrix, But use the value from LinkedList to fill the values in those matrix.</t>
   </si>
 </sst>
 </file>
@@ -206,13 +221,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -548,21 +563,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB7E3421-3FED-6D45-9062-E34708192987}">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="45" style="2" customWidth="1"/>
     <col min="2" max="2" width="86.5" customWidth="1"/>
-    <col min="3" max="3" width="61.1640625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="61.1640625" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
     </row>
@@ -605,7 +620,7 @@
       <c r="B10" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C10" s="4" t="s">
         <v>13</v>
       </c>
     </row>
@@ -616,8 +631,31 @@
       <c r="B12" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C12" s="4" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B20" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>